<commit_message>
Se agregaron jff de numeros, identificadores, comentarios. falta probar y meter tipos avanzados
</commit_message>
<xml_diff>
--- a/Proyecto/JFF/TOKENS.xlsx
+++ b/Proyecto/JFF/TOKENS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Joel\Desktop\Compi\Compiladores1\Proyecto\JFF\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DF0C18B4-CBD9-4751-B932-0854F259ECEE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95645D45-58CC-4793-8704-045357581711}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{30C21B4D-152B-4E27-9649-8E4E289B31D5}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="66">
   <si>
     <t>program</t>
   </si>
@@ -118,13 +118,127 @@
   </si>
   <si>
     <t>writeln</t>
+  </si>
+  <si>
+    <t>{}</t>
+  </si>
+  <si>
+    <t>//</t>
+  </si>
+  <si>
+    <t>(**)</t>
+  </si>
+  <si>
+    <t>[</t>
+  </si>
+  <si>
+    <t>]</t>
+  </si>
+  <si>
+    <t>,</t>
+  </si>
+  <si>
+    <t>;</t>
+  </si>
+  <si>
+    <t>Operadores</t>
+  </si>
+  <si>
+    <t>(</t>
+  </si>
+  <si>
+    <t>)</t>
+  </si>
+  <si>
+    <t>.=</t>
+  </si>
+  <si>
+    <t>.-</t>
+  </si>
+  <si>
+    <t>.+</t>
+  </si>
+  <si>
+    <t>.*</t>
+  </si>
+  <si>
+    <t>&lt;</t>
+  </si>
+  <si>
+    <t>&gt;</t>
+  </si>
+  <si>
+    <t>&lt;&gt;</t>
+  </si>
+  <si>
+    <t>&lt;=</t>
+  </si>
+  <si>
+    <t>&gt;=</t>
+  </si>
+  <si>
+    <t>Comentarios</t>
+  </si>
+  <si>
+    <t>Palabras reservadas</t>
+  </si>
+  <si>
+    <t>Constantes</t>
+  </si>
+  <si>
+    <t>Binario</t>
+  </si>
+  <si>
+    <t>Decimal</t>
+  </si>
+  <si>
+    <t>Hexadecimal</t>
+  </si>
+  <si>
+    <t>%010010</t>
+  </si>
+  <si>
+    <t>$35af</t>
+  </si>
+  <si>
+    <t>Matches</t>
+  </si>
+  <si>
+    <t>Type1</t>
+  </si>
+  <si>
+    <t>Type2</t>
+  </si>
+  <si>
+    <t>Match</t>
+  </si>
+  <si>
+    <t>Operator</t>
+  </si>
+  <si>
+    <t>Comments</t>
+  </si>
+  <si>
+    <t>Reservated</t>
+  </si>
+  <si>
+    <t>Identifiers</t>
+  </si>
+  <si>
+    <t>All</t>
+  </si>
+  <si>
+    <t>Identifier</t>
+  </si>
+  <si>
+    <t>{_}*[[a-z]|[0-9]|[_]]+</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -132,13 +246,33 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.34998626667073579"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -153,8 +287,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -469,158 +613,336 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92F05FFE-A77C-4CD3-BB7C-DDE17E6B1228}">
-  <dimension ref="C3:C30"/>
+  <dimension ref="C25:U52"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5:C7"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="73" zoomScaleNormal="73" workbookViewId="0">
+      <selection activeCell="C43" sqref="C43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="4" width="19.33203125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="3" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C3" t="s">
+    <row r="25" spans="3:21" x14ac:dyDescent="0.3">
+      <c r="C25" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D25" s="2"/>
+      <c r="E25" s="2"/>
+      <c r="F25" s="2"/>
+      <c r="G25" s="2"/>
+      <c r="H25" s="2"/>
+      <c r="I25" s="2"/>
+      <c r="J25" s="2"/>
+      <c r="K25" s="2"/>
+      <c r="L25" s="2"/>
+      <c r="M25" s="2"/>
+      <c r="N25" s="2"/>
+      <c r="O25" s="2"/>
+      <c r="P25" s="2"/>
+      <c r="Q25" s="2"/>
+    </row>
+    <row r="26" spans="3:21" x14ac:dyDescent="0.3">
+      <c r="C26" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="H26" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="I26" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="J26" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="K26" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="L26" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="M26" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="N26" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="O26" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="P26" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q26" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="28" spans="3:21" x14ac:dyDescent="0.3">
+      <c r="C28" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D28" s="2"/>
+      <c r="E28" s="2"/>
+    </row>
+    <row r="29" spans="3:21" x14ac:dyDescent="0.3">
+      <c r="C29" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="32" spans="3:21" x14ac:dyDescent="0.3">
+      <c r="C32" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D32" s="2"/>
+      <c r="E32" s="2"/>
+      <c r="F32" s="2"/>
+      <c r="G32" s="2"/>
+      <c r="H32" s="2"/>
+      <c r="I32" s="2"/>
+      <c r="J32" s="2"/>
+      <c r="K32" s="2"/>
+      <c r="L32" s="2"/>
+      <c r="M32" s="2"/>
+      <c r="N32" s="2"/>
+      <c r="O32" s="2"/>
+      <c r="P32" s="2"/>
+      <c r="Q32" s="2"/>
+      <c r="R32" s="2"/>
+      <c r="S32" s="2"/>
+      <c r="T32" s="2"/>
+      <c r="U32" s="2"/>
+    </row>
+    <row r="33" spans="3:21" x14ac:dyDescent="0.3">
+      <c r="C33" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="4" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C4" t="s">
+      <c r="D33" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G33" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H33" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="I33" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J33" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="K33" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="L33" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="M33" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="N33" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="O33" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="P33" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q33" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="R33" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="S33" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="T33" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="U33" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="34" spans="3:21" x14ac:dyDescent="0.3">
+      <c r="C34" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C5" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="6" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C6" t="s">
+      <c r="D34" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C7" t="s">
+      <c r="E34" s="1"/>
+      <c r="F34" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G34" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H34" s="1"/>
+      <c r="I34" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="J34" s="1"/>
+      <c r="K34" s="1"/>
+      <c r="L34" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="M34" s="1"/>
+      <c r="N34" s="1"/>
+      <c r="O34" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="P34" s="1"/>
+      <c r="Q34" s="1"/>
+      <c r="R34" s="1"/>
+      <c r="S34" s="1"/>
+      <c r="T34" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="U34" s="1"/>
+    </row>
+    <row r="35" spans="3:21" x14ac:dyDescent="0.3">
+      <c r="C35" s="1"/>
+      <c r="D35" s="1" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="8" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C8" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="9" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C9" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="10" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C10" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="11" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C11" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="12" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C12" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="13" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C13" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="14" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C14" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="15" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C15" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="16" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C16" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="17" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C17" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="18" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C18" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="19" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C19" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="20" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C20" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C21" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="22" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C22" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="23" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C23" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="24" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C24" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="25" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C25" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="26" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C26" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C27" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="28" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C28" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="29" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C29" t="s">
+      <c r="E35" s="1"/>
+      <c r="F35" s="1"/>
+      <c r="G35" s="1"/>
+      <c r="H35" s="1"/>
+      <c r="I35" s="1"/>
+      <c r="J35" s="1"/>
+      <c r="K35" s="1"/>
+      <c r="L35" s="1"/>
+      <c r="M35" s="1"/>
+      <c r="N35" s="1"/>
+      <c r="O35" s="1"/>
+      <c r="P35" s="1"/>
+      <c r="Q35" s="1"/>
+      <c r="R35" s="1"/>
+      <c r="S35" s="1"/>
+      <c r="T35" s="1" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="30" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C30" t="s">
-        <v>10</v>
+      <c r="U35" s="1"/>
+    </row>
+    <row r="37" spans="3:21" x14ac:dyDescent="0.3">
+      <c r="C37" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D37" s="3"/>
+      <c r="E37" s="3"/>
+      <c r="F37" s="3"/>
+    </row>
+    <row r="38" spans="3:21" x14ac:dyDescent="0.3">
+      <c r="C38" t="s">
+        <v>50</v>
+      </c>
+      <c r="D38" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="E38" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="39" spans="3:21" x14ac:dyDescent="0.3">
+      <c r="C39" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="D39">
+        <v>3215</v>
+      </c>
+      <c r="E39" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="41" spans="3:21" x14ac:dyDescent="0.3">
+      <c r="C41" s="6" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="42" spans="3:21" x14ac:dyDescent="0.3">
+      <c r="C42" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="49" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C49" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="D49" s="3"/>
+      <c r="E49" s="3"/>
+    </row>
+    <row r="50" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C50" t="s">
+        <v>56</v>
+      </c>
+      <c r="D50" t="s">
+        <v>57</v>
+      </c>
+      <c r="E50" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="51" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C51" t="s">
+        <v>59</v>
+      </c>
+      <c r="D51" t="s">
+        <v>60</v>
+      </c>
+      <c r="E51" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="52" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C52" t="s">
+        <v>61</v>
+      </c>
+      <c r="D52" t="s">
+        <v>62</v>
+      </c>
+      <c r="E52" t="s">
+        <v>63</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="C3:C30">
-    <sortCondition ref="C1:C30"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="C33:C60">
+    <sortCondition ref="C29:C60"/>
   </sortState>
+  <mergeCells count="5">
+    <mergeCell ref="C25:Q25"/>
+    <mergeCell ref="C28:E28"/>
+    <mergeCell ref="C32:U32"/>
+    <mergeCell ref="C37:F37"/>
+    <mergeCell ref="C49:E49"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>